<commit_message>
SUMMARY IS DONE WTF DO I DO NOW???????????????
</commit_message>
<xml_diff>
--- a/particleID_summary.xlsx
+++ b/particleID_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\RFID_tracers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F95DD-524F-4440-A1E1-DB91C935701D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50980CC-BF8B-4FE7-8471-BBA9549B174C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{7052B091-D471-4631-A263-E1BC3A5159A1}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{7052B091-D471-4631-A263-E1BC3A5159A1}"/>
   </bookViews>
   <sheets>
     <sheet name="RFID rock sizes" sheetId="2" r:id="rId1"/>
@@ -261,7 +261,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,12 +354,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -379,6 +373,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,9 +783,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,34 +810,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -843,37 +819,19 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -883,12 +841,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -920,10 +872,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -933,10 +885,64 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2286,30 +2292,30 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="F2" s="37" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
+      <c r="F2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="67"/>
       <c r="L2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="P2" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="39"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="67"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -2333,7 +2339,7 @@
       <c r="I3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="68" t="s">
         <v>10</v>
       </c>
       <c r="L3" s="4">
@@ -2352,7 +2358,7 @@
       <c r="R3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="40" t="s">
+      <c r="S3" s="68" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2378,7 +2384,7 @@
       <c r="I4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="41"/>
+      <c r="J4" s="69"/>
       <c r="L4" s="6">
         <v>90</v>
       </c>
@@ -2395,7 +2401,7 @@
       <c r="R4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="S4" s="41"/>
+      <c r="S4" s="69"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="18">
@@ -2473,10 +2479,10 @@
         <f>P6+1000</f>
         <v>1002</v>
       </c>
-      <c r="P6" s="26">
+      <c r="P6" s="25">
         <v>2</v>
       </c>
-      <c r="Q6" s="26">
+      <c r="Q6" s="25">
         <v>11</v>
       </c>
       <c r="R6" s="24" t="s">
@@ -2599,10 +2605,10 @@
         <f t="shared" si="0"/>
         <v>1005</v>
       </c>
-      <c r="P9" s="26">
+      <c r="P9" s="25">
         <v>5</v>
       </c>
-      <c r="Q9" s="26">
+      <c r="Q9" s="25">
         <v>16</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -2637,19 +2643,19 @@
       <c r="J10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
+      <c r="L10" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="70"/>
+      <c r="N10" s="70"/>
       <c r="O10" s="11">
         <f t="shared" si="0"/>
         <v>1006</v>
       </c>
-      <c r="P10" s="26">
+      <c r="P10" s="25">
         <v>6</v>
       </c>
-      <c r="Q10" s="26">
+      <c r="Q10" s="25">
         <v>16</v>
       </c>
       <c r="R10" s="2" t="s">
@@ -2687,10 +2693,10 @@
       <c r="L11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="35">
+      <c r="M11" s="63">
         <v>44389</v>
       </c>
-      <c r="N11" s="36"/>
+      <c r="N11" s="64"/>
       <c r="O11" s="11">
         <f t="shared" si="0"/>
         <v>1007</v>
@@ -2732,10 +2738,10 @@
       <c r="L12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="35">
+      <c r="M12" s="63">
         <v>44389</v>
       </c>
-      <c r="N12" s="36"/>
+      <c r="N12" s="64"/>
       <c r="O12" s="11">
         <f t="shared" si="0"/>
         <v>1008</v>
@@ -2777,10 +2783,10 @@
       <c r="L13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="35">
+      <c r="M13" s="63">
         <v>44389</v>
       </c>
-      <c r="N13" s="36"/>
+      <c r="N13" s="64"/>
       <c r="O13" s="11">
         <f t="shared" si="0"/>
         <v>1009</v>
@@ -2823,10 +2829,10 @@
         <f t="shared" si="0"/>
         <v>1010</v>
       </c>
-      <c r="P14" s="26">
+      <c r="P14" s="25">
         <v>10</v>
       </c>
-      <c r="Q14" s="26">
+      <c r="Q14" s="25">
         <v>16</v>
       </c>
       <c r="R14" s="3" t="s">
@@ -2861,20 +2867,20 @@
       <c r="J15" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="42" t="s">
+      <c r="L15" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="70"/>
       <c r="O15" s="11">
         <f t="shared" si="0"/>
         <v>1011</v>
       </c>
-      <c r="P15" s="26">
+      <c r="P15" s="25">
         <f>P14+1</f>
         <v>11</v>
       </c>
-      <c r="Q15" s="26">
+      <c r="Q15" s="25">
         <v>16</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -2912,10 +2918,10 @@
       <c r="L16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="35">
+      <c r="M16" s="63">
         <v>44638</v>
       </c>
-      <c r="N16" s="36"/>
+      <c r="N16" s="64"/>
       <c r="O16" s="11">
         <f t="shared" si="0"/>
         <v>1012</v>
@@ -2958,10 +2964,10 @@
       <c r="L17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="35">
+      <c r="M17" s="63">
         <v>44638</v>
       </c>
-      <c r="N17" s="36"/>
+      <c r="N17" s="64"/>
       <c r="O17" s="11">
         <f t="shared" si="0"/>
         <v>1013</v>
@@ -3005,11 +3011,11 @@
         <f t="shared" si="0"/>
         <v>1014</v>
       </c>
-      <c r="P18" s="26">
+      <c r="P18" s="25">
         <f>P17+1</f>
         <v>14</v>
       </c>
-      <c r="Q18" s="26">
+      <c r="Q18" s="25">
         <v>16</v>
       </c>
       <c r="R18" s="24" t="s">
@@ -3126,11 +3132,11 @@
         <f t="shared" si="0"/>
         <v>1017</v>
       </c>
-      <c r="P21" s="26">
+      <c r="P21" s="25">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="Q21" s="26">
+      <c r="Q21" s="25">
         <v>16</v>
       </c>
       <c r="R21" s="1" t="s">
@@ -3477,11 +3483,11 @@
         <f t="shared" si="0"/>
         <v>1026</v>
       </c>
-      <c r="P30" s="26">
+      <c r="P30" s="25">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="Q30" s="26">
+      <c r="Q30" s="25">
         <v>16</v>
       </c>
       <c r="R30" s="1" t="s">
@@ -3559,11 +3565,11 @@
         <f t="shared" si="0"/>
         <v>1028</v>
       </c>
-      <c r="P32" s="26">
+      <c r="P32" s="25">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="Q32" s="26">
+      <c r="Q32" s="25">
         <v>16</v>
       </c>
       <c r="R32" s="1" t="s">
@@ -3680,11 +3686,11 @@
         <f t="shared" si="0"/>
         <v>1031</v>
       </c>
-      <c r="P35" s="26">
+      <c r="P35" s="25">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="Q35" s="26">
+      <c r="Q35" s="25">
         <v>16</v>
       </c>
       <c r="R35" s="3" t="s">
@@ -3867,11 +3873,11 @@
         <f t="shared" si="0"/>
         <v>1036</v>
       </c>
-      <c r="P40" s="26">
+      <c r="P40" s="25">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="Q40" s="26">
+      <c r="Q40" s="25">
         <v>16</v>
       </c>
       <c r="R40" s="1" t="s">
@@ -3910,11 +3916,11 @@
         <f t="shared" si="0"/>
         <v>1037</v>
       </c>
-      <c r="P41" s="26">
+      <c r="P41" s="25">
         <f>P40+1</f>
         <v>37</v>
       </c>
-      <c r="Q41" s="26">
+      <c r="Q41" s="25">
         <v>16</v>
       </c>
       <c r="R41" s="1" t="s">
@@ -3988,11 +3994,11 @@
         <f t="shared" si="0"/>
         <v>1039</v>
       </c>
-      <c r="P43" s="26">
+      <c r="P43" s="25">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="Q43" s="26">
+      <c r="Q43" s="25">
         <v>22.6</v>
       </c>
       <c r="R43" s="3" t="s">
@@ -4031,11 +4037,11 @@
         <f t="shared" si="0"/>
         <v>1040</v>
       </c>
-      <c r="P44" s="26">
+      <c r="P44" s="25">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="Q44" s="26">
+      <c r="Q44" s="25">
         <v>22.6</v>
       </c>
       <c r="R44" s="2" t="s">
@@ -4074,11 +4080,11 @@
         <f t="shared" si="0"/>
         <v>1041</v>
       </c>
-      <c r="P45" s="26">
+      <c r="P45" s="25">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="Q45" s="26">
+      <c r="Q45" s="25">
         <v>22.6</v>
       </c>
       <c r="R45" s="24" t="s">
@@ -4117,11 +4123,11 @@
         <f t="shared" si="0"/>
         <v>1042</v>
       </c>
-      <c r="P46" s="26">
+      <c r="P46" s="25">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="Q46" s="26">
+      <c r="Q46" s="25">
         <v>22.6</v>
       </c>
       <c r="R46" s="2" t="s">
@@ -4160,11 +4166,11 @@
         <f t="shared" si="0"/>
         <v>1043</v>
       </c>
-      <c r="P47" s="26">
+      <c r="P47" s="25">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="Q47" s="26">
+      <c r="Q47" s="25">
         <v>22.6</v>
       </c>
       <c r="R47" s="24" t="s">
@@ -4203,11 +4209,11 @@
         <f t="shared" si="0"/>
         <v>1044</v>
       </c>
-      <c r="P48" s="26">
+      <c r="P48" s="25">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="Q48" s="26">
+      <c r="Q48" s="25">
         <v>22.6</v>
       </c>
       <c r="R48" s="1" t="s">
@@ -4246,11 +4252,11 @@
         <f t="shared" si="0"/>
         <v>1045</v>
       </c>
-      <c r="P49" s="26">
+      <c r="P49" s="25">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="Q49" s="26">
+      <c r="Q49" s="25">
         <v>22.6</v>
       </c>
       <c r="R49" s="24" t="s">
@@ -4324,11 +4330,11 @@
         <f t="shared" si="0"/>
         <v>1047</v>
       </c>
-      <c r="P51" s="26">
+      <c r="P51" s="25">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="Q51" s="26">
+      <c r="Q51" s="25">
         <v>22.6</v>
       </c>
       <c r="R51" s="2" t="s">
@@ -4367,11 +4373,11 @@
         <f t="shared" si="0"/>
         <v>1048</v>
       </c>
-      <c r="P52" s="26">
+      <c r="P52" s="25">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="Q52" s="26">
+      <c r="Q52" s="25">
         <v>22.6</v>
       </c>
       <c r="R52" s="2" t="s">
@@ -4410,11 +4416,11 @@
         <f t="shared" si="0"/>
         <v>1049</v>
       </c>
-      <c r="P53" s="26">
+      <c r="P53" s="25">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="Q53" s="26">
+      <c r="Q53" s="25">
         <v>22.6</v>
       </c>
       <c r="R53" s="1" t="s">
@@ -4449,11 +4455,11 @@
         <f t="shared" si="0"/>
         <v>1050</v>
       </c>
-      <c r="P54" s="26">
+      <c r="P54" s="25">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="Q54" s="26">
+      <c r="Q54" s="25">
         <v>22.6</v>
       </c>
       <c r="R54" s="1" t="s">
@@ -4492,11 +4498,11 @@
         <f t="shared" si="0"/>
         <v>1051</v>
       </c>
-      <c r="P55" s="26">
+      <c r="P55" s="25">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="Q55" s="26">
+      <c r="Q55" s="25">
         <v>22.6</v>
       </c>
       <c r="R55" s="2" t="s">
@@ -4535,11 +4541,11 @@
         <f t="shared" si="0"/>
         <v>1052</v>
       </c>
-      <c r="P56" s="26">
+      <c r="P56" s="25">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="Q56" s="26">
+      <c r="Q56" s="25">
         <v>22.6</v>
       </c>
       <c r="R56" s="1" t="s">
@@ -4578,11 +4584,11 @@
         <f t="shared" si="0"/>
         <v>1053</v>
       </c>
-      <c r="P57" s="26">
+      <c r="P57" s="25">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="Q57" s="26">
+      <c r="Q57" s="25">
         <v>22.6</v>
       </c>
       <c r="R57" s="2" t="s">
@@ -4656,11 +4662,11 @@
         <f t="shared" si="0"/>
         <v>1055</v>
       </c>
-      <c r="P59" s="26">
+      <c r="P59" s="25">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="Q59" s="26">
+      <c r="Q59" s="25">
         <v>22.6</v>
       </c>
       <c r="R59" s="1" t="s">
@@ -4735,11 +4741,11 @@
         <f t="shared" si="0"/>
         <v>1057</v>
       </c>
-      <c r="P61" s="26">
+      <c r="P61" s="25">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="Q61" s="26">
+      <c r="Q61" s="25">
         <v>22.6</v>
       </c>
       <c r="R61" s="24" t="s">
@@ -4774,11 +4780,11 @@
         <f t="shared" si="0"/>
         <v>1058</v>
       </c>
-      <c r="P62" s="26">
+      <c r="P62" s="25">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="Q62" s="26">
+      <c r="Q62" s="25">
         <v>22.6</v>
       </c>
       <c r="R62" s="24" t="s">
@@ -4896,11 +4902,11 @@
         <f t="shared" si="0"/>
         <v>1061</v>
       </c>
-      <c r="P65" s="26">
+      <c r="P65" s="25">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="Q65" s="26">
+      <c r="Q65" s="25">
         <v>22.6</v>
       </c>
       <c r="R65" s="2" t="s">
@@ -4942,11 +4948,11 @@
         <f t="shared" si="0"/>
         <v>1062</v>
       </c>
-      <c r="P66" s="26">
+      <c r="P66" s="25">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="Q66" s="26">
+      <c r="Q66" s="25">
         <v>22.6</v>
       </c>
       <c r="R66" s="2" t="s">
@@ -4985,11 +4991,11 @@
         <f t="shared" si="0"/>
         <v>1063</v>
       </c>
-      <c r="P67" s="26">
+      <c r="P67" s="25">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="Q67" s="26">
+      <c r="Q67" s="25">
         <v>22.6</v>
       </c>
       <c r="R67" s="24" t="s">
@@ -5067,11 +5073,11 @@
         <f t="shared" si="0"/>
         <v>1065</v>
       </c>
-      <c r="P69" s="26">
+      <c r="P69" s="25">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="Q69" s="26">
+      <c r="Q69" s="25">
         <v>22.6</v>
       </c>
       <c r="R69" s="1" t="s">
@@ -6939,7 +6945,7 @@
       <c r="D142" s="10">
         <v>32</v>
       </c>
-      <c r="E142" s="27" t="s">
+      <c r="E142" s="26" t="s">
         <v>15</v>
       </c>
       <c r="F142" s="1" t="s">
@@ -6954,7 +6960,7 @@
       <c r="D143" s="10">
         <v>32</v>
       </c>
-      <c r="E143" s="28" t="s">
+      <c r="E143" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F143" s="2" t="s">
@@ -6969,7 +6975,7 @@
       <c r="D144" s="10">
         <v>32</v>
       </c>
-      <c r="E144" s="29" t="s">
+      <c r="E144" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F144" s="3" t="s">
@@ -6999,7 +7005,7 @@
       <c r="D146" s="10">
         <v>32</v>
       </c>
-      <c r="E146" s="28" t="s">
+      <c r="E146" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F146" s="2" t="s">
@@ -7014,7 +7020,7 @@
       <c r="D147" s="10">
         <v>32</v>
       </c>
-      <c r="E147" s="29" t="s">
+      <c r="E147" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F147" s="3" t="s">
@@ -7044,7 +7050,7 @@
       <c r="D149" s="10">
         <v>32</v>
       </c>
-      <c r="E149" s="29" t="s">
+      <c r="E149" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F149" s="3" t="s">
@@ -7059,7 +7065,7 @@
       <c r="D150" s="10">
         <v>32</v>
       </c>
-      <c r="E150" s="28" t="s">
+      <c r="E150" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F150" s="2" t="s">
@@ -7074,7 +7080,7 @@
       <c r="D151" s="10">
         <v>32</v>
       </c>
-      <c r="E151" s="29" t="s">
+      <c r="E151" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F151" s="3" t="s">
@@ -7104,7 +7110,7 @@
       <c r="D153" s="10">
         <v>32</v>
       </c>
-      <c r="E153" s="28" t="s">
+      <c r="E153" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F153" s="2" t="s">
@@ -7112,14 +7118,14 @@
       </c>
     </row>
     <row r="154" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B154" s="30">
+      <c r="B154" s="29">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="D154" s="6">
         <v>90</v>
       </c>
-      <c r="E154" s="27" t="s">
+      <c r="E154" s="26" t="s">
         <v>15</v>
       </c>
       <c r="F154" s="1" t="s">
@@ -7127,7 +7133,7 @@
       </c>
     </row>
     <row r="155" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B155" s="30">
+      <c r="B155" s="29">
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
@@ -7142,14 +7148,14 @@
       </c>
     </row>
     <row r="156" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B156" s="30">
+      <c r="B156" s="29">
         <f t="shared" si="2"/>
         <v>152</v>
       </c>
       <c r="D156" s="6">
         <v>90</v>
       </c>
-      <c r="E156" s="29" t="s">
+      <c r="E156" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F156" s="3" t="s">
@@ -7157,7 +7163,7 @@
       </c>
     </row>
     <row r="157" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B157" s="30">
+      <c r="B157" s="29">
         <f t="shared" si="2"/>
         <v>153</v>
       </c>
@@ -7172,14 +7178,14 @@
       </c>
     </row>
     <row r="158" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B158" s="30">
+      <c r="B158" s="29">
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
       <c r="D158" s="6">
         <v>90</v>
       </c>
-      <c r="E158" s="28" t="s">
+      <c r="E158" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F158" s="2" t="s">
@@ -7187,14 +7193,14 @@
       </c>
     </row>
     <row r="159" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B159" s="30">
+      <c r="B159" s="29">
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="D159" s="6">
         <v>90</v>
       </c>
-      <c r="E159" s="29" t="s">
+      <c r="E159" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F159" s="3" t="s">
@@ -7202,14 +7208,14 @@
       </c>
     </row>
     <row r="160" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B160" s="30">
+      <c r="B160" s="29">
         <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="D160" s="6">
         <v>90</v>
       </c>
-      <c r="E160" s="27" t="s">
+      <c r="E160" s="26" t="s">
         <v>15</v>
       </c>
       <c r="F160" s="1" t="s">
@@ -7217,14 +7223,14 @@
       </c>
     </row>
     <row r="161" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B161" s="30">
+      <c r="B161" s="29">
         <f t="shared" si="2"/>
         <v>157</v>
       </c>
       <c r="D161" s="6">
         <v>90</v>
       </c>
-      <c r="E161" s="27" t="s">
+      <c r="E161" s="26" t="s">
         <v>15</v>
       </c>
       <c r="F161" s="1" t="s">
@@ -7239,7 +7245,7 @@
       <c r="D162" s="9">
         <v>45</v>
       </c>
-      <c r="E162" s="28" t="s">
+      <c r="E162" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F162" s="2" t="s">
@@ -7269,7 +7275,7 @@
       <c r="D164" s="9">
         <v>45</v>
       </c>
-      <c r="E164" s="29" t="s">
+      <c r="E164" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F164" s="3" t="s">
@@ -7299,7 +7305,7 @@
       <c r="D166" s="9">
         <v>45</v>
       </c>
-      <c r="E166" s="29" t="s">
+      <c r="E166" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F166" s="3" t="s">
@@ -7329,7 +7335,7 @@
       <c r="D168" s="9">
         <v>45</v>
       </c>
-      <c r="E168" s="28" t="s">
+      <c r="E168" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F168" s="2" t="s">
@@ -7337,14 +7343,14 @@
       </c>
     </row>
     <row r="169" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B169" s="31">
+      <c r="B169" s="30">
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
-      <c r="D169" s="43">
-        <v>16</v>
-      </c>
-      <c r="E169" s="27" t="s">
+      <c r="D169" s="34">
+        <v>16</v>
+      </c>
+      <c r="E169" s="26" t="s">
         <v>15</v>
       </c>
       <c r="F169" s="1" t="s">
@@ -7352,14 +7358,14 @@
       </c>
     </row>
     <row r="170" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B170" s="31">
+      <c r="B170" s="30">
         <f t="shared" si="2"/>
         <v>166</v>
       </c>
-      <c r="D170" s="43">
-        <v>16</v>
-      </c>
-      <c r="E170" s="27" t="s">
+      <c r="D170" s="34">
+        <v>16</v>
+      </c>
+      <c r="E170" s="26" t="s">
         <v>15</v>
       </c>
       <c r="F170" s="1" t="s">
@@ -7387,7 +7393,7 @@
       <c r="D172" s="4">
         <v>128</v>
       </c>
-      <c r="E172" s="29" t="s">
+      <c r="E172" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F172" s="3" t="s">
@@ -7401,7 +7407,7 @@
       <c r="D173" s="4">
         <v>128</v>
       </c>
-      <c r="E173" s="28" t="s">
+      <c r="E173" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F173" s="2" t="s">
@@ -7416,7 +7422,7 @@
       <c r="D174" s="8">
         <v>64</v>
       </c>
-      <c r="E174" s="29" t="s">
+      <c r="E174" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F174" s="3" t="s">
@@ -7435,7 +7441,7 @@
       <c r="B176" s="11">
         <v>1002</v>
       </c>
-      <c r="D176" s="26">
+      <c r="D176" s="25">
         <v>11</v>
       </c>
     </row>
@@ -7459,7 +7465,7 @@
       <c r="B179" s="11">
         <v>1005</v>
       </c>
-      <c r="D179" s="26">
+      <c r="D179" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7467,7 +7473,7 @@
       <c r="B180" s="11">
         <v>1006</v>
       </c>
-      <c r="D180" s="26">
+      <c r="D180" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7499,7 +7505,7 @@
       <c r="B184" s="11">
         <v>1010</v>
       </c>
-      <c r="D184" s="26">
+      <c r="D184" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7507,7 +7513,7 @@
       <c r="B185" s="11">
         <v>1011</v>
       </c>
-      <c r="D185" s="26">
+      <c r="D185" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7531,7 +7537,7 @@
       <c r="B188" s="11">
         <v>1014</v>
       </c>
-      <c r="D188" s="26">
+      <c r="D188" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7555,7 +7561,7 @@
       <c r="B191" s="11">
         <v>1017</v>
       </c>
-      <c r="D191" s="26">
+      <c r="D191" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7627,7 +7633,7 @@
       <c r="B200" s="11">
         <v>1026</v>
       </c>
-      <c r="D200" s="26">
+      <c r="D200" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7643,7 +7649,7 @@
       <c r="B202" s="11">
         <v>1028</v>
       </c>
-      <c r="D202" s="26">
+      <c r="D202" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7667,7 +7673,7 @@
       <c r="B205" s="11">
         <v>1031</v>
       </c>
-      <c r="D205" s="26">
+      <c r="D205" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7707,7 +7713,7 @@
       <c r="B210" s="11">
         <v>1036</v>
       </c>
-      <c r="D210" s="26">
+      <c r="D210" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7715,7 +7721,7 @@
       <c r="B211" s="11">
         <v>1037</v>
       </c>
-      <c r="D211" s="26">
+      <c r="D211" s="25">
         <v>16</v>
       </c>
     </row>
@@ -7731,7 +7737,7 @@
       <c r="B213" s="11">
         <v>1039</v>
       </c>
-      <c r="D213" s="26">
+      <c r="D213" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7739,7 +7745,7 @@
       <c r="B214" s="11">
         <v>1040</v>
       </c>
-      <c r="D214" s="26">
+      <c r="D214" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7747,7 +7753,7 @@
       <c r="B215" s="11">
         <v>1041</v>
       </c>
-      <c r="D215" s="26">
+      <c r="D215" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7755,7 +7761,7 @@
       <c r="B216" s="11">
         <v>1042</v>
       </c>
-      <c r="D216" s="26">
+      <c r="D216" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7763,7 +7769,7 @@
       <c r="B217" s="11">
         <v>1043</v>
       </c>
-      <c r="D217" s="26">
+      <c r="D217" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7771,7 +7777,7 @@
       <c r="B218" s="11">
         <v>1044</v>
       </c>
-      <c r="D218" s="26">
+      <c r="D218" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7779,7 +7785,7 @@
       <c r="B219" s="11">
         <v>1045</v>
       </c>
-      <c r="D219" s="26">
+      <c r="D219" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7795,7 +7801,7 @@
       <c r="B221" s="11">
         <v>1047</v>
       </c>
-      <c r="D221" s="26">
+      <c r="D221" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7803,7 +7809,7 @@
       <c r="B222" s="11">
         <v>1048</v>
       </c>
-      <c r="D222" s="26">
+      <c r="D222" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7811,7 +7817,7 @@
       <c r="B223" s="11">
         <v>1049</v>
       </c>
-      <c r="D223" s="26">
+      <c r="D223" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7819,7 +7825,7 @@
       <c r="B224" s="11">
         <v>1050</v>
       </c>
-      <c r="D224" s="26">
+      <c r="D224" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7827,7 +7833,7 @@
       <c r="B225" s="11">
         <v>1051</v>
       </c>
-      <c r="D225" s="26">
+      <c r="D225" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7835,7 +7841,7 @@
       <c r="B226" s="11">
         <v>1052</v>
       </c>
-      <c r="D226" s="26">
+      <c r="D226" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7843,7 +7849,7 @@
       <c r="B227" s="11">
         <v>1053</v>
       </c>
-      <c r="D227" s="26">
+      <c r="D227" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7859,7 +7865,7 @@
       <c r="B229" s="11">
         <v>1055</v>
       </c>
-      <c r="D229" s="26">
+      <c r="D229" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7875,7 +7881,7 @@
       <c r="B231" s="11">
         <v>1057</v>
       </c>
-      <c r="D231" s="26">
+      <c r="D231" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7883,7 +7889,7 @@
       <c r="B232" s="11">
         <v>1058</v>
       </c>
-      <c r="D232" s="26">
+      <c r="D232" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7907,7 +7913,7 @@
       <c r="B235" s="11">
         <v>1061</v>
       </c>
-      <c r="D235" s="26">
+      <c r="D235" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7915,7 +7921,7 @@
       <c r="B236" s="11">
         <v>1062</v>
       </c>
-      <c r="D236" s="26">
+      <c r="D236" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7923,7 +7929,7 @@
       <c r="B237" s="11">
         <v>1063</v>
       </c>
-      <c r="D237" s="26">
+      <c r="D237" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7939,7 +7945,7 @@
       <c r="B239" s="11">
         <v>1065</v>
       </c>
-      <c r="D239" s="26">
+      <c r="D239" s="25">
         <v>22.6</v>
       </c>
     </row>
@@ -7974,8 +7980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2DDA353-7660-4CD7-8317-1897C5DB3F0B}">
   <dimension ref="A1:B204"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R179" sqref="R179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7988,7 +7994,7 @@
       <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7996,7 +8002,7 @@
       <c r="A2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>24</v>
       </c>
     </row>
@@ -9089,530 +9095,530 @@
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="44">
+      <c r="A139" s="79">
         <v>22.6</v>
       </c>
-      <c r="B139" s="25">
+      <c r="B139" s="80">
         <v>1039</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="44">
+      <c r="A140" s="79">
         <v>22.6</v>
       </c>
-      <c r="B140" s="25">
+      <c r="B140" s="80">
         <v>1040</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="44">
+      <c r="A141" s="79">
         <v>22.6</v>
       </c>
-      <c r="B141" s="25">
+      <c r="B141" s="80">
         <v>1041</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="44">
+      <c r="A142" s="79">
         <v>22.6</v>
       </c>
-      <c r="B142" s="25">
+      <c r="B142" s="80">
         <v>1042</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="44">
+      <c r="A143" s="79">
         <v>22.6</v>
       </c>
-      <c r="B143" s="25">
+      <c r="B143" s="80">
         <v>1043</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="44">
+      <c r="A144" s="79">
         <v>22.6</v>
       </c>
-      <c r="B144" s="25">
+      <c r="B144" s="80">
         <v>1044</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="44">
+      <c r="A145" s="79">
         <v>22.6</v>
       </c>
-      <c r="B145" s="25">
+      <c r="B145" s="80">
         <v>1045</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="44">
+      <c r="A146" s="79">
         <v>22.6</v>
       </c>
-      <c r="B146" s="25">
+      <c r="B146" s="80">
         <v>1046</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="44">
+      <c r="A147" s="79">
         <v>22.6</v>
       </c>
-      <c r="B147" s="25">
+      <c r="B147" s="80">
         <v>1047</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="44">
+      <c r="A148" s="79">
         <v>22.6</v>
       </c>
-      <c r="B148" s="25">
+      <c r="B148" s="80">
         <v>1048</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="44">
+      <c r="A149" s="79">
         <v>22.6</v>
       </c>
-      <c r="B149" s="25">
+      <c r="B149" s="80">
         <v>1049</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="44">
+      <c r="A150" s="79">
         <v>22.6</v>
       </c>
-      <c r="B150" s="25">
+      <c r="B150" s="80">
         <v>1050</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="44">
+      <c r="A151" s="79">
         <v>22.6</v>
       </c>
-      <c r="B151" s="25">
+      <c r="B151" s="80">
         <v>1051</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="44">
+      <c r="A152" s="79">
         <v>22.6</v>
       </c>
-      <c r="B152" s="25">
+      <c r="B152" s="80">
         <v>1052</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="44">
+      <c r="A153" s="79">
         <v>22.6</v>
       </c>
-      <c r="B153" s="25">
+      <c r="B153" s="80">
         <v>1053</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="44">
+      <c r="A154" s="79">
         <v>22.6</v>
       </c>
-      <c r="B154" s="25">
+      <c r="B154" s="80">
         <v>1054</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="44">
+      <c r="A155" s="79">
         <v>22.6</v>
       </c>
-      <c r="B155" s="25">
+      <c r="B155" s="80">
         <v>1055</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="44">
+      <c r="A156" s="79">
         <v>22.6</v>
       </c>
-      <c r="B156" s="25">
+      <c r="B156" s="80">
         <v>1056</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="44">
+      <c r="A157" s="79">
         <v>22.6</v>
       </c>
-      <c r="B157" s="25">
+      <c r="B157" s="80">
         <v>1057</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="44">
+      <c r="A158" s="79">
         <v>22.6</v>
       </c>
-      <c r="B158" s="25">
+      <c r="B158" s="80">
         <v>1058</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="44">
+      <c r="A159" s="79">
         <v>22.6</v>
       </c>
-      <c r="B159" s="25">
+      <c r="B159" s="80">
         <v>1059</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="44">
+      <c r="A160" s="79">
         <v>22.6</v>
       </c>
-      <c r="B160" s="25">
+      <c r="B160" s="80">
         <v>1060</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="44">
+      <c r="A161" s="79">
         <v>22.6</v>
       </c>
-      <c r="B161" s="25">
+      <c r="B161" s="80">
         <v>1061</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="44">
+      <c r="A162" s="79">
         <v>22.6</v>
       </c>
-      <c r="B162" s="25">
+      <c r="B162" s="80">
         <v>1062</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="44">
+      <c r="A163" s="79">
         <v>22.6</v>
       </c>
-      <c r="B163" s="25">
+      <c r="B163" s="80">
         <v>1063</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="44">
+      <c r="A164" s="79">
         <v>22.6</v>
       </c>
-      <c r="B164" s="25">
+      <c r="B164" s="80">
         <v>1064</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="44">
+      <c r="A165" s="79">
         <v>22.6</v>
       </c>
-      <c r="B165" s="25">
+      <c r="B165" s="80">
         <v>1065</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="44">
+      <c r="A166" s="79">
         <v>22.6</v>
       </c>
-      <c r="B166" s="25">
+      <c r="B166" s="80">
         <v>1066</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="45">
-        <v>16</v>
-      </c>
-      <c r="B167" s="46">
+      <c r="A167" s="81">
+        <v>16</v>
+      </c>
+      <c r="B167" s="82">
         <v>1004</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="45">
-        <v>16</v>
-      </c>
-      <c r="B168" s="46">
+      <c r="A168" s="81">
+        <v>16</v>
+      </c>
+      <c r="B168" s="82">
         <v>1005</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="45">
-        <v>16</v>
-      </c>
-      <c r="B169" s="46">
+      <c r="A169" s="81">
+        <v>16</v>
+      </c>
+      <c r="B169" s="82">
         <v>1006</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="45">
-        <v>16</v>
-      </c>
-      <c r="B170" s="46">
+      <c r="A170" s="81">
+        <v>16</v>
+      </c>
+      <c r="B170" s="82">
         <v>1007</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="45">
-        <v>16</v>
-      </c>
-      <c r="B171" s="46">
+      <c r="A171" s="81">
+        <v>16</v>
+      </c>
+      <c r="B171" s="82">
         <v>1008</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="45">
-        <v>16</v>
-      </c>
-      <c r="B172" s="46">
+      <c r="A172" s="81">
+        <v>16</v>
+      </c>
+      <c r="B172" s="82">
         <v>1009</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="45">
-        <v>16</v>
-      </c>
-      <c r="B173" s="46">
+      <c r="A173" s="81">
+        <v>16</v>
+      </c>
+      <c r="B173" s="82">
         <v>1010</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="45">
-        <v>16</v>
-      </c>
-      <c r="B174" s="46">
+      <c r="A174" s="81">
+        <v>16</v>
+      </c>
+      <c r="B174" s="82">
         <v>1011</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="45">
-        <v>16</v>
-      </c>
-      <c r="B175" s="46">
+      <c r="A175" s="81">
+        <v>16</v>
+      </c>
+      <c r="B175" s="82">
         <v>1012</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="45">
-        <v>16</v>
-      </c>
-      <c r="B176" s="46">
+      <c r="A176" s="81">
+        <v>16</v>
+      </c>
+      <c r="B176" s="82">
         <v>1013</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="45">
-        <v>16</v>
-      </c>
-      <c r="B177" s="46">
+      <c r="A177" s="81">
+        <v>16</v>
+      </c>
+      <c r="B177" s="82">
         <v>1014</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="45">
-        <v>16</v>
-      </c>
-      <c r="B178" s="46">
+      <c r="A178" s="81">
+        <v>16</v>
+      </c>
+      <c r="B178" s="82">
         <v>1015</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="45">
-        <v>16</v>
-      </c>
-      <c r="B179" s="46">
+      <c r="A179" s="81">
+        <v>16</v>
+      </c>
+      <c r="B179" s="82">
         <v>1016</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="45">
-        <v>16</v>
-      </c>
-      <c r="B180" s="46">
+      <c r="A180" s="81">
+        <v>16</v>
+      </c>
+      <c r="B180" s="82">
         <v>1017</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="45">
-        <v>16</v>
-      </c>
-      <c r="B181" s="46">
+      <c r="A181" s="81">
+        <v>16</v>
+      </c>
+      <c r="B181" s="82">
         <v>1018</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="45">
-        <v>16</v>
-      </c>
-      <c r="B182" s="46">
+      <c r="A182" s="81">
+        <v>16</v>
+      </c>
+      <c r="B182" s="82">
         <v>1019</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="45">
-        <v>16</v>
-      </c>
-      <c r="B183" s="46">
+      <c r="A183" s="81">
+        <v>16</v>
+      </c>
+      <c r="B183" s="82">
         <v>1020</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="45">
-        <v>16</v>
-      </c>
-      <c r="B184" s="46">
+      <c r="A184" s="81">
+        <v>16</v>
+      </c>
+      <c r="B184" s="82">
         <v>1021</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="45">
-        <v>16</v>
-      </c>
-      <c r="B185" s="46">
+      <c r="A185" s="81">
+        <v>16</v>
+      </c>
+      <c r="B185" s="82">
         <v>1022</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="45">
-        <v>16</v>
-      </c>
-      <c r="B186" s="46">
+      <c r="A186" s="81">
+        <v>16</v>
+      </c>
+      <c r="B186" s="82">
         <v>1023</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="45">
-        <v>16</v>
-      </c>
-      <c r="B187" s="46">
+      <c r="A187" s="81">
+        <v>16</v>
+      </c>
+      <c r="B187" s="82">
         <v>1024</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="45">
-        <v>16</v>
-      </c>
-      <c r="B188" s="46">
+      <c r="A188" s="81">
+        <v>16</v>
+      </c>
+      <c r="B188" s="82">
         <v>1025</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="45">
-        <v>16</v>
-      </c>
-      <c r="B189" s="46">
+      <c r="A189" s="81">
+        <v>16</v>
+      </c>
+      <c r="B189" s="82">
         <v>1026</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="45">
-        <v>16</v>
-      </c>
-      <c r="B190" s="46">
+      <c r="A190" s="81">
+        <v>16</v>
+      </c>
+      <c r="B190" s="82">
         <v>1027</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="45">
-        <v>16</v>
-      </c>
-      <c r="B191" s="46">
+      <c r="A191" s="81">
+        <v>16</v>
+      </c>
+      <c r="B191" s="82">
         <v>1028</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="45">
-        <v>16</v>
-      </c>
-      <c r="B192" s="46">
+      <c r="A192" s="81">
+        <v>16</v>
+      </c>
+      <c r="B192" s="82">
         <v>1029</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="45">
-        <v>16</v>
-      </c>
-      <c r="B193" s="46">
+      <c r="A193" s="81">
+        <v>16</v>
+      </c>
+      <c r="B193" s="82">
         <v>1030</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="45">
-        <v>16</v>
-      </c>
-      <c r="B194" s="46">
+      <c r="A194" s="81">
+        <v>16</v>
+      </c>
+      <c r="B194" s="82">
         <v>1031</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="45">
-        <v>16</v>
-      </c>
-      <c r="B195" s="46">
+      <c r="A195" s="81">
+        <v>16</v>
+      </c>
+      <c r="B195" s="82">
         <v>1032</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="45">
-        <v>16</v>
-      </c>
-      <c r="B196" s="46">
+      <c r="A196" s="81">
+        <v>16</v>
+      </c>
+      <c r="B196" s="82">
         <v>1033</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="45">
-        <v>16</v>
-      </c>
-      <c r="B197" s="46">
+      <c r="A197" s="81">
+        <v>16</v>
+      </c>
+      <c r="B197" s="82">
         <v>1034</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="45">
-        <v>16</v>
-      </c>
-      <c r="B198" s="46">
+      <c r="A198" s="81">
+        <v>16</v>
+      </c>
+      <c r="B198" s="82">
         <v>1035</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="45">
-        <v>16</v>
-      </c>
-      <c r="B199" s="46">
+      <c r="A199" s="81">
+        <v>16</v>
+      </c>
+      <c r="B199" s="82">
         <v>1036</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="45">
-        <v>16</v>
-      </c>
-      <c r="B200" s="46">
+      <c r="A200" s="81">
+        <v>16</v>
+      </c>
+      <c r="B200" s="82">
         <v>1037</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="45">
-        <v>16</v>
-      </c>
-      <c r="B201" s="46">
+      <c r="A201" s="81">
+        <v>16</v>
+      </c>
+      <c r="B201" s="82">
         <v>1038</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="47">
+      <c r="A202" s="35">
         <v>11</v>
       </c>
-      <c r="B202" s="48">
+      <c r="B202" s="36">
         <v>1001</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="47">
+      <c r="A203" s="35">
         <v>11</v>
       </c>
-      <c r="B203" s="48">
+      <c r="B203" s="36">
         <v>1002</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="47">
+      <c r="A204" s="35">
         <v>11</v>
       </c>
-      <c r="B204" s="48">
+      <c r="B204" s="36">
         <v>1003</v>
       </c>
     </row>
@@ -9625,7 +9631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BB005D-B354-4E22-ADBC-5647CCDA417C}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
@@ -9638,432 +9644,432 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="F1" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="57"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="F1" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="74"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61" t="s">
+      <c r="H2" s="44"/>
+      <c r="I2" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="62"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="38">
         <v>10</v>
       </c>
-      <c r="C3" s="52">
+      <c r="C3" s="39">
         <v>0</v>
       </c>
-      <c r="D3" s="53">
+      <c r="D3" s="40">
         <v>0</v>
       </c>
-      <c r="F3" s="63">
+      <c r="F3" s="45">
         <f>D11</f>
         <v>31.753554502369667</v>
       </c>
-      <c r="G3" s="32">
-        <v>45</v>
-      </c>
-      <c r="H3" s="60"/>
-      <c r="I3" s="32" t="s">
+      <c r="G3" s="31">
+        <v>45</v>
+      </c>
+      <c r="H3" s="44"/>
+      <c r="I3" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="64">
+      <c r="J3" s="46">
         <f>F3</f>
         <v>31.753554502369667</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="51">
+      <c r="A4" s="38">
         <v>4</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="38">
         <v>0</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="38">
         <v>0</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="41">
         <v>0</v>
       </c>
-      <c r="F4" s="63">
+      <c r="F4" s="45">
         <v>52.132701421800952</v>
       </c>
-      <c r="G4" s="32">
-        <v>64</v>
-      </c>
-      <c r="H4" s="60"/>
-      <c r="I4" s="32" t="s">
+      <c r="G4" s="31">
+        <v>64</v>
+      </c>
+      <c r="H4" s="44"/>
+      <c r="I4" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="65">
+      <c r="J4" s="47">
         <f>G3</f>
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="51">
+      <c r="A5" s="38">
         <v>5.6</v>
       </c>
-      <c r="B5" s="51">
+      <c r="B5" s="38">
         <v>0</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="38">
         <v>0</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="41">
         <v>0</v>
       </c>
-      <c r="F5" s="66">
+      <c r="F5" s="48">
         <v>50</v>
       </c>
-      <c r="G5" s="67">
+      <c r="G5" s="49">
         <f>J8</f>
         <v>62.011627906976742</v>
       </c>
-      <c r="H5" s="60"/>
-      <c r="I5" s="32" t="s">
+      <c r="H5" s="44"/>
+      <c r="I5" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="64">
+      <c r="J5" s="46">
         <f>F4</f>
         <v>52.132701421800952</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51">
+      <c r="A6" s="38">
         <v>8</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="38">
         <v>0</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="38">
         <v>0</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="41">
         <v>0</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="32" t="s">
+      <c r="F6" s="50"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="65">
+      <c r="J6" s="47">
         <f>G4</f>
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51">
+      <c r="A7" s="38">
         <v>11</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="38">
         <v>5</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="38">
         <v>0</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="41">
         <v>0</v>
       </c>
-      <c r="F7" s="69" t="s">
+      <c r="F7" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="70">
+      <c r="G7" s="52">
         <f>G5</f>
         <v>62.011627906976742</v>
       </c>
-      <c r="H7" s="71" t="s">
+      <c r="H7" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="72" t="s">
+      <c r="I7" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="65">
+      <c r="J7" s="47">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51">
-        <v>16</v>
-      </c>
-      <c r="B8" s="51">
+      <c r="A8" s="38">
+        <v>16</v>
+      </c>
+      <c r="B8" s="38">
         <v>10</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="38">
         <v>5</v>
       </c>
-      <c r="D8" s="54">
+      <c r="D8" s="41">
         <v>2.3696682464454977</v>
       </c>
-      <c r="F8" s="73"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="76" t="s">
+      <c r="F8" s="55"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="77">
+      <c r="J8" s="59">
         <f>J4+(J7-J3)*(J6-J4)/(J5-J3)</f>
         <v>62.011627906976742</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51">
+      <c r="A9" s="38">
         <v>22.6</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B9" s="38">
         <v>25</v>
       </c>
-      <c r="C9" s="51">
-        <v>15</v>
-      </c>
-      <c r="D9" s="54">
+      <c r="C9" s="38">
+        <v>15</v>
+      </c>
+      <c r="D9" s="41">
         <v>7.109004739336493</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51">
-        <v>32</v>
-      </c>
-      <c r="B10" s="51">
+      <c r="A10" s="38">
+        <v>32</v>
+      </c>
+      <c r="B10" s="38">
         <v>27</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="38">
         <v>40</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="41">
         <v>18.957345971563981</v>
       </c>
-      <c r="F10" s="55" t="s">
+      <c r="F10" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="57"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="74"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="51">
-        <v>45</v>
-      </c>
-      <c r="B11" s="51">
+      <c r="A11" s="38">
+        <v>45</v>
+      </c>
+      <c r="B11" s="38">
         <v>43</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="38">
         <v>67</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="41">
         <v>31.753554502369667</v>
       </c>
-      <c r="F11" s="78" t="s">
+      <c r="F11" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="80"/>
-      <c r="I11" s="81" t="s">
+      <c r="H11" s="62"/>
+      <c r="I11" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="82"/>
+      <c r="J11" s="78"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="51">
-        <v>64</v>
-      </c>
-      <c r="B12" s="51">
+      <c r="A12" s="38">
+        <v>64</v>
+      </c>
+      <c r="B12" s="38">
         <v>43</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="38">
         <v>110</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="41">
         <v>52.132701421800952</v>
       </c>
-      <c r="F12" s="63">
+      <c r="F12" s="45">
         <f>D13</f>
         <v>72.511848341232238</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="31">
         <f>A13</f>
         <v>90</v>
       </c>
-      <c r="H12" s="60"/>
-      <c r="I12" s="32" t="s">
+      <c r="H12" s="44"/>
+      <c r="I12" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="64">
+      <c r="J12" s="46">
         <f>F12</f>
         <v>72.511848341232238</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="51">
+      <c r="A13" s="38">
         <v>90</v>
       </c>
-      <c r="B13" s="51">
+      <c r="B13" s="38">
         <v>35</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="38">
         <v>153</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="41">
         <v>72.511848341232238</v>
       </c>
-      <c r="F13" s="63">
+      <c r="F13" s="45">
         <f>D14</f>
         <v>89.099526066350705</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="31">
         <f>A14</f>
         <v>128</v>
       </c>
-      <c r="H13" s="60"/>
-      <c r="I13" s="32" t="s">
+      <c r="H13" s="44"/>
+      <c r="I13" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="65">
+      <c r="J13" s="47">
         <f>G12</f>
         <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="51">
+      <c r="A14" s="38">
         <v>128</v>
       </c>
-      <c r="B14" s="51">
+      <c r="B14" s="38">
         <v>10</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="38">
         <v>188</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="41">
         <v>89.099526066350705</v>
       </c>
-      <c r="F14" s="66">
+      <c r="F14" s="48">
         <v>84</v>
       </c>
-      <c r="G14" s="67">
+      <c r="G14" s="49">
         <f>J17</f>
         <v>116.31771428571429</v>
       </c>
-      <c r="H14" s="60"/>
-      <c r="I14" s="32" t="s">
+      <c r="H14" s="44"/>
+      <c r="I14" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="64">
+      <c r="J14" s="46">
         <f>F13</f>
         <v>89.099526066350705</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="51">
+      <c r="A15" s="38">
         <v>180</v>
       </c>
-      <c r="B15" s="51">
+      <c r="B15" s="38">
         <v>13</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C15" s="38">
         <v>198</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="41">
         <v>93.838862559241704</v>
       </c>
-      <c r="F15" s="68"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="32" t="s">
+      <c r="F15" s="50"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="65">
+      <c r="J15" s="47">
         <f>G13</f>
         <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51">
+      <c r="A16" s="38">
         <v>256</v>
       </c>
-      <c r="B16" s="51">
+      <c r="B16" s="38">
         <v>0</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="38">
         <v>211</v>
       </c>
-      <c r="D16" s="54">
+      <c r="D16" s="41">
         <v>100</v>
       </c>
-      <c r="F16" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="70">
+      <c r="F16" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="52">
         <f>G14</f>
         <v>116.31771428571429</v>
       </c>
-      <c r="H16" s="71" t="s">
+      <c r="H16" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="72" t="s">
+      <c r="I16" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="65">
+      <c r="J16" s="47">
         <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="51">
+      <c r="B17" s="38">
         <v>211</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="38">
         <v>211</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="76" t="s">
+      <c r="D17" s="38"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="77">
+      <c r="J17" s="59">
         <f>J13+(J16-J12)*(J15-J13)/(J14-J12)</f>
         <v>116.31771428571429</v>
       </c>

</xml_diff>

<commit_message>
particle ID groups for sebs
</commit_message>
<xml_diff>
--- a/particleID_summary.xlsx
+++ b/particleID_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\RFID_tracers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50980CC-BF8B-4FE7-8471-BBA9549B174C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51DBBE1-44F7-4711-B1C9-00FC1F12A4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{7052B091-D471-4631-A263-E1BC3A5159A1}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{7052B091-D471-4631-A263-E1BC3A5159A1}"/>
   </bookViews>
   <sheets>
     <sheet name="RFID rock sizes" sheetId="2" r:id="rId1"/>
@@ -885,6 +885,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -931,18 +943,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2265,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BFDF8F-F407-4400-858A-9062197B06F7}">
   <dimension ref="B1:S240"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N163" sqref="N163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,30 +2292,30 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="67"/>
-      <c r="F2" s="65" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="F2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="67"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
       <c r="L2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="65" t="s">
+      <c r="P2" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="67"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="71"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -2339,7 +2339,7 @@
       <c r="I3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="68" t="s">
+      <c r="J3" s="72" t="s">
         <v>10</v>
       </c>
       <c r="L3" s="4">
@@ -2358,7 +2358,7 @@
       <c r="R3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="68" t="s">
+      <c r="S3" s="72" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2384,7 +2384,7 @@
       <c r="I4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="69"/>
+      <c r="J4" s="73"/>
       <c r="L4" s="6">
         <v>90</v>
       </c>
@@ -2401,7 +2401,7 @@
       <c r="R4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="S4" s="69"/>
+      <c r="S4" s="73"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="18">
@@ -2643,11 +2643,11 @@
       <c r="J10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="70" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="70"/>
-      <c r="N10" s="70"/>
+      <c r="L10" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
       <c r="O10" s="11">
         <f t="shared" si="0"/>
         <v>1006</v>
@@ -2693,10 +2693,10 @@
       <c r="L11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="63">
+      <c r="M11" s="67">
         <v>44389</v>
       </c>
-      <c r="N11" s="64"/>
+      <c r="N11" s="68"/>
       <c r="O11" s="11">
         <f t="shared" si="0"/>
         <v>1007</v>
@@ -2738,10 +2738,10 @@
       <c r="L12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="63">
+      <c r="M12" s="67">
         <v>44389</v>
       </c>
-      <c r="N12" s="64"/>
+      <c r="N12" s="68"/>
       <c r="O12" s="11">
         <f t="shared" si="0"/>
         <v>1008</v>
@@ -2783,10 +2783,10 @@
       <c r="L13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="63">
+      <c r="M13" s="67">
         <v>44389</v>
       </c>
-      <c r="N13" s="64"/>
+      <c r="N13" s="68"/>
       <c r="O13" s="11">
         <f t="shared" si="0"/>
         <v>1009</v>
@@ -2867,11 +2867,11 @@
       <c r="J15" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="70" t="s">
+      <c r="L15" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="70"/>
-      <c r="N15" s="70"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="74"/>
       <c r="O15" s="11">
         <f t="shared" si="0"/>
         <v>1011</v>
@@ -2918,10 +2918,10 @@
       <c r="L16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="63">
+      <c r="M16" s="67">
         <v>44638</v>
       </c>
-      <c r="N16" s="64"/>
+      <c r="N16" s="68"/>
       <c r="O16" s="11">
         <f t="shared" si="0"/>
         <v>1012</v>
@@ -2964,10 +2964,10 @@
       <c r="L17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="63">
+      <c r="M17" s="67">
         <v>44638</v>
       </c>
-      <c r="N17" s="64"/>
+      <c r="N17" s="68"/>
       <c r="O17" s="11">
         <f t="shared" si="0"/>
         <v>1013</v>
@@ -7980,7 +7980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2DDA353-7660-4CD7-8317-1897C5DB3F0B}">
   <dimension ref="A1:B204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A168" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R179" sqref="R179"/>
     </sheetView>
   </sheetViews>
@@ -9095,506 +9095,506 @@
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="79">
+      <c r="A139" s="63">
         <v>22.6</v>
       </c>
-      <c r="B139" s="80">
+      <c r="B139" s="64">
         <v>1039</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="79">
+      <c r="A140" s="63">
         <v>22.6</v>
       </c>
-      <c r="B140" s="80">
+      <c r="B140" s="64">
         <v>1040</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="79">
+      <c r="A141" s="63">
         <v>22.6</v>
       </c>
-      <c r="B141" s="80">
+      <c r="B141" s="64">
         <v>1041</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="79">
+      <c r="A142" s="63">
         <v>22.6</v>
       </c>
-      <c r="B142" s="80">
+      <c r="B142" s="64">
         <v>1042</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="79">
+      <c r="A143" s="63">
         <v>22.6</v>
       </c>
-      <c r="B143" s="80">
+      <c r="B143" s="64">
         <v>1043</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="79">
+      <c r="A144" s="63">
         <v>22.6</v>
       </c>
-      <c r="B144" s="80">
+      <c r="B144" s="64">
         <v>1044</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="79">
+      <c r="A145" s="63">
         <v>22.6</v>
       </c>
-      <c r="B145" s="80">
+      <c r="B145" s="64">
         <v>1045</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="79">
+      <c r="A146" s="63">
         <v>22.6</v>
       </c>
-      <c r="B146" s="80">
+      <c r="B146" s="64">
         <v>1046</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="79">
+      <c r="A147" s="63">
         <v>22.6</v>
       </c>
-      <c r="B147" s="80">
+      <c r="B147" s="64">
         <v>1047</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="79">
+      <c r="A148" s="63">
         <v>22.6</v>
       </c>
-      <c r="B148" s="80">
+      <c r="B148" s="64">
         <v>1048</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="79">
+      <c r="A149" s="63">
         <v>22.6</v>
       </c>
-      <c r="B149" s="80">
+      <c r="B149" s="64">
         <v>1049</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="79">
+      <c r="A150" s="63">
         <v>22.6</v>
       </c>
-      <c r="B150" s="80">
+      <c r="B150" s="64">
         <v>1050</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="79">
+      <c r="A151" s="63">
         <v>22.6</v>
       </c>
-      <c r="B151" s="80">
+      <c r="B151" s="64">
         <v>1051</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="79">
+      <c r="A152" s="63">
         <v>22.6</v>
       </c>
-      <c r="B152" s="80">
+      <c r="B152" s="64">
         <v>1052</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="79">
+      <c r="A153" s="63">
         <v>22.6</v>
       </c>
-      <c r="B153" s="80">
+      <c r="B153" s="64">
         <v>1053</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="79">
+      <c r="A154" s="63">
         <v>22.6</v>
       </c>
-      <c r="B154" s="80">
+      <c r="B154" s="64">
         <v>1054</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="79">
+      <c r="A155" s="63">
         <v>22.6</v>
       </c>
-      <c r="B155" s="80">
+      <c r="B155" s="64">
         <v>1055</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="79">
+      <c r="A156" s="63">
         <v>22.6</v>
       </c>
-      <c r="B156" s="80">
+      <c r="B156" s="64">
         <v>1056</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="79">
+      <c r="A157" s="63">
         <v>22.6</v>
       </c>
-      <c r="B157" s="80">
+      <c r="B157" s="64">
         <v>1057</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="79">
+      <c r="A158" s="63">
         <v>22.6</v>
       </c>
-      <c r="B158" s="80">
+      <c r="B158" s="64">
         <v>1058</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="79">
+      <c r="A159" s="63">
         <v>22.6</v>
       </c>
-      <c r="B159" s="80">
+      <c r="B159" s="64">
         <v>1059</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="79">
+      <c r="A160" s="63">
         <v>22.6</v>
       </c>
-      <c r="B160" s="80">
+      <c r="B160" s="64">
         <v>1060</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="79">
+      <c r="A161" s="63">
         <v>22.6</v>
       </c>
-      <c r="B161" s="80">
+      <c r="B161" s="64">
         <v>1061</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="79">
+      <c r="A162" s="63">
         <v>22.6</v>
       </c>
-      <c r="B162" s="80">
+      <c r="B162" s="64">
         <v>1062</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="79">
+      <c r="A163" s="63">
         <v>22.6</v>
       </c>
-      <c r="B163" s="80">
+      <c r="B163" s="64">
         <v>1063</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="79">
+      <c r="A164" s="63">
         <v>22.6</v>
       </c>
-      <c r="B164" s="80">
+      <c r="B164" s="64">
         <v>1064</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="79">
+      <c r="A165" s="63">
         <v>22.6</v>
       </c>
-      <c r="B165" s="80">
+      <c r="B165" s="64">
         <v>1065</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="79">
+      <c r="A166" s="63">
         <v>22.6</v>
       </c>
-      <c r="B166" s="80">
+      <c r="B166" s="64">
         <v>1066</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="81">
-        <v>16</v>
-      </c>
-      <c r="B167" s="82">
+      <c r="A167" s="65">
+        <v>16</v>
+      </c>
+      <c r="B167" s="66">
         <v>1004</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="81">
-        <v>16</v>
-      </c>
-      <c r="B168" s="82">
+      <c r="A168" s="65">
+        <v>16</v>
+      </c>
+      <c r="B168" s="66">
         <v>1005</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="81">
-        <v>16</v>
-      </c>
-      <c r="B169" s="82">
+      <c r="A169" s="65">
+        <v>16</v>
+      </c>
+      <c r="B169" s="66">
         <v>1006</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="81">
-        <v>16</v>
-      </c>
-      <c r="B170" s="82">
+      <c r="A170" s="65">
+        <v>16</v>
+      </c>
+      <c r="B170" s="66">
         <v>1007</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="81">
-        <v>16</v>
-      </c>
-      <c r="B171" s="82">
+      <c r="A171" s="65">
+        <v>16</v>
+      </c>
+      <c r="B171" s="66">
         <v>1008</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="81">
-        <v>16</v>
-      </c>
-      <c r="B172" s="82">
+      <c r="A172" s="65">
+        <v>16</v>
+      </c>
+      <c r="B172" s="66">
         <v>1009</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="81">
-        <v>16</v>
-      </c>
-      <c r="B173" s="82">
+      <c r="A173" s="65">
+        <v>16</v>
+      </c>
+      <c r="B173" s="66">
         <v>1010</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="81">
-        <v>16</v>
-      </c>
-      <c r="B174" s="82">
+      <c r="A174" s="65">
+        <v>16</v>
+      </c>
+      <c r="B174" s="66">
         <v>1011</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="81">
-        <v>16</v>
-      </c>
-      <c r="B175" s="82">
+      <c r="A175" s="65">
+        <v>16</v>
+      </c>
+      <c r="B175" s="66">
         <v>1012</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="81">
-        <v>16</v>
-      </c>
-      <c r="B176" s="82">
+      <c r="A176" s="65">
+        <v>16</v>
+      </c>
+      <c r="B176" s="66">
         <v>1013</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="81">
-        <v>16</v>
-      </c>
-      <c r="B177" s="82">
+      <c r="A177" s="65">
+        <v>16</v>
+      </c>
+      <c r="B177" s="66">
         <v>1014</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="81">
-        <v>16</v>
-      </c>
-      <c r="B178" s="82">
+      <c r="A178" s="65">
+        <v>16</v>
+      </c>
+      <c r="B178" s="66">
         <v>1015</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="81">
-        <v>16</v>
-      </c>
-      <c r="B179" s="82">
+      <c r="A179" s="65">
+        <v>16</v>
+      </c>
+      <c r="B179" s="66">
         <v>1016</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="81">
-        <v>16</v>
-      </c>
-      <c r="B180" s="82">
+      <c r="A180" s="65">
+        <v>16</v>
+      </c>
+      <c r="B180" s="66">
         <v>1017</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="81">
-        <v>16</v>
-      </c>
-      <c r="B181" s="82">
+      <c r="A181" s="65">
+        <v>16</v>
+      </c>
+      <c r="B181" s="66">
         <v>1018</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="81">
-        <v>16</v>
-      </c>
-      <c r="B182" s="82">
+      <c r="A182" s="65">
+        <v>16</v>
+      </c>
+      <c r="B182" s="66">
         <v>1019</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="81">
-        <v>16</v>
-      </c>
-      <c r="B183" s="82">
+      <c r="A183" s="65">
+        <v>16</v>
+      </c>
+      <c r="B183" s="66">
         <v>1020</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="81">
-        <v>16</v>
-      </c>
-      <c r="B184" s="82">
+      <c r="A184" s="65">
+        <v>16</v>
+      </c>
+      <c r="B184" s="66">
         <v>1021</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="81">
-        <v>16</v>
-      </c>
-      <c r="B185" s="82">
+      <c r="A185" s="65">
+        <v>16</v>
+      </c>
+      <c r="B185" s="66">
         <v>1022</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="81">
-        <v>16</v>
-      </c>
-      <c r="B186" s="82">
+      <c r="A186" s="65">
+        <v>16</v>
+      </c>
+      <c r="B186" s="66">
         <v>1023</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="81">
-        <v>16</v>
-      </c>
-      <c r="B187" s="82">
+      <c r="A187" s="65">
+        <v>16</v>
+      </c>
+      <c r="B187" s="66">
         <v>1024</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="81">
-        <v>16</v>
-      </c>
-      <c r="B188" s="82">
+      <c r="A188" s="65">
+        <v>16</v>
+      </c>
+      <c r="B188" s="66">
         <v>1025</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="81">
-        <v>16</v>
-      </c>
-      <c r="B189" s="82">
+      <c r="A189" s="65">
+        <v>16</v>
+      </c>
+      <c r="B189" s="66">
         <v>1026</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="81">
-        <v>16</v>
-      </c>
-      <c r="B190" s="82">
+      <c r="A190" s="65">
+        <v>16</v>
+      </c>
+      <c r="B190" s="66">
         <v>1027</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="81">
-        <v>16</v>
-      </c>
-      <c r="B191" s="82">
+      <c r="A191" s="65">
+        <v>16</v>
+      </c>
+      <c r="B191" s="66">
         <v>1028</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="81">
-        <v>16</v>
-      </c>
-      <c r="B192" s="82">
+      <c r="A192" s="65">
+        <v>16</v>
+      </c>
+      <c r="B192" s="66">
         <v>1029</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="81">
-        <v>16</v>
-      </c>
-      <c r="B193" s="82">
+      <c r="A193" s="65">
+        <v>16</v>
+      </c>
+      <c r="B193" s="66">
         <v>1030</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="81">
-        <v>16</v>
-      </c>
-      <c r="B194" s="82">
+      <c r="A194" s="65">
+        <v>16</v>
+      </c>
+      <c r="B194" s="66">
         <v>1031</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="81">
-        <v>16</v>
-      </c>
-      <c r="B195" s="82">
+      <c r="A195" s="65">
+        <v>16</v>
+      </c>
+      <c r="B195" s="66">
         <v>1032</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="81">
-        <v>16</v>
-      </c>
-      <c r="B196" s="82">
+      <c r="A196" s="65">
+        <v>16</v>
+      </c>
+      <c r="B196" s="66">
         <v>1033</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="81">
-        <v>16</v>
-      </c>
-      <c r="B197" s="82">
+      <c r="A197" s="65">
+        <v>16</v>
+      </c>
+      <c r="B197" s="66">
         <v>1034</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="81">
-        <v>16</v>
-      </c>
-      <c r="B198" s="82">
+      <c r="A198" s="65">
+        <v>16</v>
+      </c>
+      <c r="B198" s="66">
         <v>1035</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="81">
-        <v>16</v>
-      </c>
-      <c r="B199" s="82">
+      <c r="A199" s="65">
+        <v>16</v>
+      </c>
+      <c r="B199" s="66">
         <v>1036</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="81">
-        <v>16</v>
-      </c>
-      <c r="B200" s="82">
+      <c r="A200" s="65">
+        <v>16</v>
+      </c>
+      <c r="B200" s="66">
         <v>1037</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="81">
-        <v>16</v>
-      </c>
-      <c r="B201" s="82">
+      <c r="A201" s="65">
+        <v>16</v>
+      </c>
+      <c r="B201" s="66">
         <v>1038</v>
       </c>
     </row>
@@ -9644,19 +9644,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="F1" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="F1" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="78"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
@@ -9678,10 +9678,10 @@
         <v>34</v>
       </c>
       <c r="H2" s="44"/>
-      <c r="I2" s="75" t="s">
+      <c r="I2" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="76"/>
+      <c r="J2" s="80"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
@@ -9876,13 +9876,13 @@
       <c r="D10" s="41">
         <v>18.957345971563981</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="74"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="78"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
@@ -9904,10 +9904,10 @@
         <v>34</v>
       </c>
       <c r="H11" s="62"/>
-      <c r="I11" s="77" t="s">
+      <c r="I11" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="78"/>
+      <c r="J11" s="82"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="38">

</xml_diff>